<commit_message>
【 Project - UART_controller 】 Change to reference 3 TX and RX design
</commit_message>
<xml_diff>
--- a/Project - Uart_controller/De10_UART_controller.xlsx
+++ b/Project - Uart_controller/De10_UART_controller.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intelFPGA_lite\18.1\Digital-Clock\Project - Simple_UART_controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intelFPGA_lite\18.1\Digital-Clock\Project - Uart_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF6F1F9-D0BC-45C3-A4D5-F8A54F5E90F2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1FCCB6-FF75-4D1A-92D0-8439A1718C58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{8B4AF6FD-1216-4FEA-B286-4A054EDE5B68}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>1.</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>https://www.circuitbasics.com/basics-uart-communication/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Wsou_zhCEYQ</t>
+  </si>
+  <si>
+    <t>3.</t>
   </si>
 </sst>
 </file>
@@ -788,146 +794,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>102219</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>144037</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>306657</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>130098</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="53" name="Group 52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F11BBB4-2391-4B16-80D6-07AD2C08CE84}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1934960" y="3954037"/>
-          <a:ext cx="815352" cy="1129061"/>
-          <a:chOff x="1988635" y="4000500"/>
-          <a:chExt cx="613316" cy="938561"/>
-        </a:xfrm>
-        <a:solidFill>
-          <a:srgbClr val="00B0F0"/>
-        </a:solidFill>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="51" name="Rectangle 50">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1E11A15-ED40-4B6A-B710-B28C3293772F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1988635" y="4000500"/>
-            <a:ext cx="613316" cy="938561"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:grpFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-MY" sz="1100"/>
-              <a:t>Baud Rate Generator</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="52" name="Isosceles Triangle 51">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{738A20E0-0E5C-4810-B398-4F27B1B2BCE6}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="5400000">
-            <a:off x="1974695" y="4595232"/>
-            <a:ext cx="226369" cy="195146"/>
-          </a:xfrm>
-          <a:prstGeom prst="triangle">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-MY" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>240680</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -1298,11 +1164,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>483220</xdr:colOff>
+      <xdr:colOff>105104</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>170055</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="676509" cy="264560"/>
+    <xdr:ext cx="1054626" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="68" name="TextBox 67">
@@ -1316,8 +1182,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4135244" y="3599055"/>
-          <a:ext cx="676509" cy="264560"/>
+          <a:off x="3770587" y="3599055"/>
+          <a:ext cx="1054626" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1346,7 +1212,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-MY" sz="1100"/>
-            <a:t>rx_done</a:t>
+            <a:t>data_available</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1471,216 +1337,6 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>483219</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>73414</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>240680</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>74342</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="74" name="Straight Arrow Connector 73">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98F4543B-03B3-41EB-8002-1C10A0104E59}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="55" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2917902" y="3883414"/>
-          <a:ext cx="366132" cy="928"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>487866</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>69695</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>487866</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>120805</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="77" name="Straight Connector 76">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EC9DD88-D1A9-4461-B2BC-6C842B6F2432}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2922549" y="3879695"/>
-          <a:ext cx="0" cy="1003610"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>505522</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114302</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>262983</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>115229</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="Straight Arrow Connector 77">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BA90FA6-C1EB-49A5-BB0E-C232E1382381}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2940205" y="4876802"/>
-          <a:ext cx="366132" cy="927"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>311305</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>55756</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>501805</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>55756</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="82" name="Straight Connector 81">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6A651E-811A-4887-8CFB-4858136BF3D1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2745988" y="4437256"/>
-          <a:ext cx="190500" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>199792</xdr:colOff>
       <xdr:row>19</xdr:row>
@@ -2848,11 +2504,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>602167</xdr:colOff>
+      <xdr:colOff>98534</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>79915</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="531542" cy="264560"/>
+    <xdr:ext cx="1035175" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="123" name="TextBox 122">
@@ -2866,8 +2522,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4254191" y="5032915"/>
-          <a:ext cx="531542" cy="264560"/>
+          <a:off x="3764017" y="5223415"/>
+          <a:ext cx="1035175" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2896,7 +2552,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-MY" sz="1100"/>
-            <a:t>tx_go</a:t>
+            <a:t>data_available</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4651,8 +4307,8 @@
       <xdr:rowOff>26276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>91965</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>26276</xdr:rowOff>
     </xdr:to>
@@ -4670,7 +4326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1188983" y="4788776"/>
-          <a:ext cx="735723" cy="0"/>
+          <a:ext cx="1872155" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4700,8 +4356,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>295603</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19707</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>86710</xdr:rowOff>
     </xdr:from>
@@ -4709,7 +4365,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>237795</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>86710</xdr:rowOff>
+      <xdr:rowOff>91966</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4723,9 +4379,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1517431" y="5611210"/>
-          <a:ext cx="1774933" cy="0"/>
+        <a:xfrm flipV="1">
+          <a:off x="3074276" y="5611210"/>
+          <a:ext cx="218088" cy="5256"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -5166,61 +4822,6 @@
         <a:xfrm>
           <a:off x="5127737" y="4198883"/>
           <a:ext cx="0" cy="366548"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:srgbClr val="F117D2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>294292</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>28904</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>294292</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>65690</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="190" name="Straight Connector 189">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319C5FB6-302A-4FA4-98E2-036AC9383197}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1516120" y="4791404"/>
-          <a:ext cx="0" cy="798786"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -5622,7 +5223,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5638,7 +5239,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5663,13 +5264,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{960063BA-F99D-4CAF-B621-E727AE01726F}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{A68908B6-3565-4819-A150-681FF468015D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
【 Project - UART_controller 】 Add in new module and change display method
1. Add in FIFO 8bit data size 10 depth
2. change display method, any data received will save in FIFO, tx will sent the data in same FIFO
</commit_message>
<xml_diff>
--- a/Project - Uart_controller/De10_UART_controller.xlsx
+++ b/Project - Uart_controller/De10_UART_controller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intelFPGA_lite\18.1\Digital-Clock\Project - Uart_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1FCCB6-FF75-4D1A-92D0-8439A1718C58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FA0411-F497-4D03-9B10-C77DACD81EE8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{8B4AF6FD-1216-4FEA-B286-4A054EDE5B68}"/>
   </bookViews>
@@ -647,7 +647,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>571499</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>14868</xdr:rowOff>
+      <xdr:rowOff>177362</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -663,7 +663,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="1681814" y="2836078"/>
-          <a:ext cx="5609737" cy="3084290"/>
+          <a:ext cx="5609737" cy="3246784"/>
           <a:chOff x="1626147" y="240820"/>
           <a:chExt cx="1727966" cy="1854680"/>
         </a:xfrm>
@@ -991,8 +991,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>258337</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>89211</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>78828</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1007,8 +1007,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5260588" y="4675150"/>
-          <a:ext cx="1084456" cy="938561"/>
+          <a:off x="5889446" y="4865650"/>
+          <a:ext cx="1088943" cy="1118678"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1878,9 +1878,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>78058</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>126379</xdr:rowOff>
+      <xdr:colOff>84627</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>34414</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="648629" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -1896,7 +1896,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5556095" y="3936379"/>
+          <a:off x="6193765" y="3463414"/>
           <a:ext cx="648629" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2678,9 +2678,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>146824</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>106864</xdr:rowOff>
+      <xdr:colOff>100841</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>179123</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="648629" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -2696,7 +2696,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5624861" y="5250364"/>
+          <a:off x="6209979" y="4941623"/>
           <a:ext cx="648629" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2740,7 +2740,7 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>75269</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="611325" cy="264560"/>
+    <xdr:ext cx="839702" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="127" name="TextBox 126">
@@ -2754,8 +2754,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5861957" y="5218769"/>
-          <a:ext cx="611325" cy="264560"/>
+          <a:off x="5873781" y="5218769"/>
+          <a:ext cx="839702" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2784,7 +2784,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-MY" sz="1100"/>
-            <a:t>empty</a:t>
+            <a:t>data_ready</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3124,7 +3124,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>526381</xdr:colOff>
+      <xdr:colOff>526382</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>17049</xdr:rowOff>
     </xdr:from>
@@ -3132,7 +3132,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>375557</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>17049</xdr:rowOff>
+      <xdr:rowOff>17050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3149,8 +3149,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4793581" y="5351049"/>
-          <a:ext cx="1068376" cy="0"/>
+          <a:off x="4802779" y="5351049"/>
+          <a:ext cx="1071002" cy="1"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3177,142 +3177,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>600307</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>89210</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>218005</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>157427</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="133" name="Isosceles Triangle 132">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD429862-CED6-4AC7-B417-A15221CD0CC2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="4844828" y="5058384"/>
-          <a:ext cx="258717" cy="226369"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B0F0"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-MY" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>497158</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171915</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>576146</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>60403</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="134" name="Oval 133">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CFAAF64-ECDD-4F21-A874-A7AE6F2D672D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4757853" y="5124915"/>
-          <a:ext cx="78988" cy="78988"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B0F0"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-MY" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -4920,6 +4784,288 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>357163</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>148840</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="877802" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="87" name="TextBox 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91B3FA01-F16B-4C41-A9F0-F37810C3C0B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5855387" y="5673340"/>
+          <a:ext cx="877802" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1100"/>
+            <a:t>empty</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>413845</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>105105</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>385033</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>105105</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="88" name="Straight Connector 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B68AB82-4DEC-4458-BF44-8B6D97B4C657}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5301155" y="5820105"/>
+          <a:ext cx="582102" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>423137</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>115934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>423137</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>88055</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="Straight Connector 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01113CC2-A71B-4808-BC11-25FA938759F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5310447" y="5830934"/>
+          <a:ext cx="0" cy="543621"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>432430</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>92702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>472966</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>92702</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="Straight Arrow Connector 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF0989B6-0967-4DD8-82D4-1E46C252174A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5319740" y="6379202"/>
+          <a:ext cx="3095105" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>446690</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>124810</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1270314" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="TextBox 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5AA9190-0D88-4B6A-A828-28E4A890053D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8388569" y="6220810"/>
+          <a:ext cx="1270314" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1100"/>
+            <a:t>tx_empty</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5223,7 +5369,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>